<commit_message>
Edit PMP,SRS,CR, and Time plan
</commit_message>
<xml_diff>
--- a/project_management/Change Requests.xlsx
+++ b/project_management/Change Requests.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -25,16 +25,40 @@
     <t>Impact</t>
   </si>
   <si>
+    <t>Analysis</t>
+  </si>
+  <si>
     <t>Action</t>
   </si>
   <si>
     <t>Status</t>
   </si>
   <si>
+    <t>Inititation Date</t>
+  </si>
+  <si>
+    <t>Completion Date</t>
+  </si>
+  <si>
     <t>CR_01</t>
   </si>
   <si>
+    <t xml:space="preserve"> remove admin features from the project.</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>no impact on other classes</t>
+  </si>
+  <si>
+    <t>removal of the class</t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
   <si>
     <t>CR_02</t>
@@ -68,6 +92,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m-d-yyyy"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10.0"/>
@@ -107,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -118,6 +145,12 @@
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -336,12 +369,14 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="23.13"/>
+    <col customWidth="1" min="2" max="2" width="74.13"/>
     <col customWidth="1" min="3" max="3" width="18.63"/>
     <col customWidth="1" min="4" max="4" width="13.75"/>
-    <col customWidth="1" min="5" max="5" width="16.13"/>
-    <col customWidth="1" min="6" max="6" width="17.75"/>
-    <col customWidth="1" min="7" max="7" width="25.5"/>
+    <col customWidth="1" min="5" max="5" width="31.88"/>
+    <col customWidth="1" min="6" max="6" width="26.5"/>
+    <col customWidth="1" min="7" max="7" width="17.75"/>
+    <col customWidth="1" min="8" max="8" width="25.5"/>
+    <col customWidth="1" min="9" max="9" width="32.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -363,85 +398,112 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="5">
+        <v>45601.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>